<commit_message>
adjust the table position
</commit_message>
<xml_diff>
--- a/winter_paralympics.xlsx
+++ b/winter_paralympics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9024" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9024"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_of _data_1" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -904,7 +904,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -915,6 +915,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -927,21 +943,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" pivotButton="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" pivotButton="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="10" xfId="21" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" pivotButton="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -988,94 +991,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="25">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFA7D00"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="65"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7F7F7F"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
+      <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFA7D00"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="65"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF7F7F7F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF7F7F7F"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF7F7F7F"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
+      <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
       </font>
     </dxf>
     <dxf>
@@ -1117,262 +1042,6 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="65"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1440,13 +1109,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -1747,46 +1409,6 @@
             </a:effectLst>
           </c:spPr>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
@@ -1828,46 +1450,6 @@
             </a:effectLst>
           </c:spPr>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -2159,11 +1741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-888324544"/>
-        <c:axId val="-888316928"/>
+        <c:axId val="-497877024"/>
+        <c:axId val="-497867232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-888324544"/>
+        <c:axId val="-497877024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +1860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-888316928"/>
+        <c:crossAx val="-497867232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2286,7 +1868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-888316928"/>
+        <c:axId val="-497867232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2347,7 +1929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-888324544"/>
+        <c:crossAx val="-497877024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8483,7 +8065,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="34" rowHeaderCaption="Years">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="34" rowHeaderCaption="Years">
   <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
@@ -8663,11 +8245,29 @@
     <dataField name="Participeted_Country" fld="3" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of M_Total" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="40">
+  <formats count="3">
+    <format dxfId="24">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
         </references>
       </pivotArea>
     </format>
@@ -8720,7 +8320,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="Hosted_country">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="Hosted_country">
   <location ref="A3:L65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -9054,17 +8654,17 @@
     <dataField name="Participated_country" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="22">
-    <format dxfId="38">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="21">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1" selected="0">
@@ -9073,16 +8673,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="20">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="I1" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="18">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="50">
@@ -9140,7 +8740,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="11">
@@ -9159,29 +8759,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="13">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="12">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="11">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -9190,7 +8790,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -9199,7 +8799,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -9208,7 +8808,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="7">
@@ -9219,122 +8819,6 @@
             <x v="7"/>
             <x v="8"/>
             <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="50">
-            <x v="0"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="8"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-            <x v="13"/>
-            <x v="14"/>
-            <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
-            <x v="18"/>
-            <x v="19"/>
-            <x v="20"/>
-            <x v="21"/>
-            <x v="22"/>
-            <x v="23"/>
-            <x v="24"/>
-            <x v="25"/>
-            <x v="26"/>
-            <x v="27"/>
-            <x v="28"/>
-            <x v="31"/>
-            <x v="33"/>
-            <x v="35"/>
-            <x v="36"/>
-            <x v="37"/>
-            <x v="38"/>
-            <x v="39"/>
-            <x v="40"/>
-            <x v="41"/>
-            <x v="43"/>
-            <x v="45"/>
-            <x v="47"/>
-            <x v="48"/>
-            <x v="49"/>
-            <x v="50"/>
-            <x v="51"/>
-            <x v="52"/>
-            <x v="54"/>
-            <x v="55"/>
-            <x v="56"/>
-            <x v="57"/>
-            <x v="58"/>
-            <x v="59"/>
-            <x v="60"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="50">
-            <x v="0"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="8"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-            <x v="13"/>
-            <x v="14"/>
-            <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
-            <x v="18"/>
-            <x v="19"/>
-            <x v="20"/>
-            <x v="21"/>
-            <x v="22"/>
-            <x v="23"/>
-            <x v="24"/>
-            <x v="25"/>
-            <x v="26"/>
-            <x v="27"/>
-            <x v="28"/>
-            <x v="31"/>
-            <x v="33"/>
-            <x v="35"/>
-            <x v="36"/>
-            <x v="37"/>
-            <x v="38"/>
-            <x v="39"/>
-            <x v="40"/>
-            <x v="41"/>
-            <x v="43"/>
-            <x v="45"/>
-            <x v="47"/>
-            <x v="48"/>
-            <x v="49"/>
-            <x v="50"/>
-            <x v="51"/>
-            <x v="52"/>
-            <x v="54"/>
-            <x v="55"/>
-            <x v="56"/>
-            <x v="57"/>
-            <x v="58"/>
-            <x v="59"/>
-            <x v="60"/>
           </reference>
         </references>
       </pivotArea>
@@ -9397,7 +8881,123 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="50">
+            <x v="0"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="8"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+            <x v="15"/>
+            <x v="16"/>
+            <x v="17"/>
+            <x v="18"/>
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+            <x v="25"/>
+            <x v="26"/>
+            <x v="27"/>
+            <x v="28"/>
+            <x v="31"/>
+            <x v="33"/>
+            <x v="35"/>
+            <x v="36"/>
+            <x v="37"/>
+            <x v="38"/>
+            <x v="39"/>
+            <x v="40"/>
+            <x v="41"/>
+            <x v="43"/>
+            <x v="45"/>
+            <x v="47"/>
+            <x v="48"/>
+            <x v="49"/>
+            <x v="50"/>
+            <x v="51"/>
+            <x v="52"/>
+            <x v="54"/>
+            <x v="55"/>
+            <x v="56"/>
+            <x v="57"/>
+            <x v="58"/>
+            <x v="59"/>
+            <x v="60"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="50">
+            <x v="0"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="8"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+            <x v="15"/>
+            <x v="16"/>
+            <x v="17"/>
+            <x v="18"/>
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+            <x v="25"/>
+            <x v="26"/>
+            <x v="27"/>
+            <x v="28"/>
+            <x v="31"/>
+            <x v="33"/>
+            <x v="35"/>
+            <x v="36"/>
+            <x v="37"/>
+            <x v="38"/>
+            <x v="39"/>
+            <x v="40"/>
+            <x v="41"/>
+            <x v="43"/>
+            <x v="45"/>
+            <x v="47"/>
+            <x v="48"/>
+            <x v="49"/>
+            <x v="50"/>
+            <x v="51"/>
+            <x v="52"/>
+            <x v="54"/>
+            <x v="55"/>
+            <x v="56"/>
+            <x v="57"/>
+            <x v="58"/>
+            <x v="59"/>
+            <x v="60"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="11">
@@ -9691,15 +9291,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" customWidth="1"/>
@@ -9713,35 +9313,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="F2" s="8" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
@@ -9890,8 +9490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="92" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView zoomScale="92" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9906,7 +9506,7 @@
     <col min="8" max="8" width="15.88671875" customWidth="1"/>
     <col min="9" max="9" width="6.21875" customWidth="1"/>
     <col min="10" max="10" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="22.109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="22.109375" style="7" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.109375" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
@@ -10022,1869 +9622,1869 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>114</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>11</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>20</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="8">
         <v>14</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>34</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>57</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="8">
         <v>7</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="8">
         <v>11</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>35</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="8">
         <v>29</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="10">
         <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="8">
         <v>101</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>6</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>14</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="8">
         <v>5</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>40</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>118</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="8">
         <v>8</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="8">
         <v>4</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>12</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="8">
         <v>19</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="10">
         <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="8">
         <v>65</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>13</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>45</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>12</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>34</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>49</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="8">
         <v>36</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="8">
         <v>18</v>
       </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11">
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
         <v>43</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="10">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8">
         <v>24</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>38</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="8">
         <v>18</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>44</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>64</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="8">
         <v>19</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="8">
         <v>15</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8">
         <v>33</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="10">
         <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8">
         <v>38</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8">
         <v>33</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>31</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>30</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8">
         <v>80</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11">
+      <c r="J9" s="8"/>
+      <c r="K9" s="8">
         <v>21</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="10">
         <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="8">
         <v>59</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>2</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>14</v>
       </c>
-      <c r="E10" s="11">
-        <v>0</v>
-      </c>
-      <c r="F10" s="11">
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
         <v>19</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>59</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="8">
         <v>3</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="8">
         <v>1</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <v>22</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="8">
         <v>8</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="10">
         <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="8">
         <v>19</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>6</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>19</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>15</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>22</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>34</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="8">
         <v>20</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="8">
         <v>12</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>5</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="8">
         <v>19</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="10">
         <v>171</v>
       </c>
-      <c r="O11" s="10"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="8">
         <v>27</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>19</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>12</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="8">
         <v>13</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>15</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="8">
         <v>14</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="8">
         <v>28</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="8">
         <v>16</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>4</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="8">
         <v>15</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="10">
         <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="8">
         <v>60</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
         <v>3</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <v>15</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="8">
         <v>2</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>23</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <v>26</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="8">
         <v>3</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="8">
         <v>1</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="8">
         <v>12</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="8">
         <v>12</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="10">
         <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8">
         <v>19</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8">
         <v>25</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <v>9</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8">
         <v>22</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="8">
         <v>25</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11">
+      <c r="J14" s="8"/>
+      <c r="K14" s="8">
         <v>12</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="10">
         <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="8">
         <v>64</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
         <v>18</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11">
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8">
         <v>28</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="13">
+      <c r="K15" s="8"/>
+      <c r="L15" s="10">
         <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="8">
         <v>29</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <v>2</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <v>4</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="8">
         <v>1</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <v>6</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="8">
         <v>24</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="8">
         <v>1</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="8">
         <v>4</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="8">
         <v>20</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="8">
         <v>9</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="10">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="8">
         <v>2</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>11</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="8">
         <v>2</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="8">
         <v>9</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>41</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="8">
         <v>6</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="8">
         <v>10</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="8">
         <v>6</v>
       </c>
-      <c r="J17" s="11">
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
         <v>3</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="10">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="8">
         <v>10</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
         <v>7</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="8">
         <v>4</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="8">
         <v>8</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <v>10</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="8">
         <v>13</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="8">
         <v>5</v>
       </c>
-      <c r="I18" s="11">
-        <v>0</v>
-      </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11">
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8">
         <v>9</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="10">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8">
         <v>11</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8">
         <v>2</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="8">
         <v>10</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <v>5</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="8">
         <v>11</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="8">
         <v>7</v>
       </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11">
+      <c r="J19" s="8"/>
+      <c r="K19" s="8">
         <v>9</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="10">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="8">
         <v>21</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <v>1</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="8">
         <v>5</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="8">
         <v>2</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8">
         <v>2</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="8">
         <v>10</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="8">
         <v>1</v>
       </c>
-      <c r="I20" s="11">
-        <v>0</v>
-      </c>
-      <c r="J20" s="11">
-        <v>0</v>
-      </c>
-      <c r="K20" s="11">
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0</v>
+      </c>
+      <c r="K20" s="8">
         <v>3</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="10">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="8">
         <v>4</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="8">
         <v>3</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="8">
         <v>4</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="8">
         <v>2</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="8">
         <v>8</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="8">
         <v>10</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="8">
         <v>2</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="8">
         <v>3</v>
       </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11">
+      <c r="J21" s="8"/>
+      <c r="K21" s="8">
         <v>7</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="10">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8">
         <v>9</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8">
         <v>9</v>
       </c>
-      <c r="F22" s="11">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <v>0</v>
-      </c>
-      <c r="H22" s="11">
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
         <v>12</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="8">
         <v>3</v>
       </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8">
         <v>2</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="10">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="8">
         <v>10</v>
       </c>
-      <c r="C23" s="11">
-        <v>0</v>
-      </c>
-      <c r="D23" s="11">
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8">
         <v>5</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="8">
         <v>1</v>
       </c>
-      <c r="F23" s="11">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
         <v>5</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="8">
         <v>7</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="8">
         <v>6</v>
       </c>
-      <c r="J23" s="11">
-        <v>0</v>
-      </c>
-      <c r="K23" s="11">
-        <v>0</v>
-      </c>
-      <c r="L23" s="13">
+      <c r="J23" s="8">
+        <v>0</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0</v>
+      </c>
+      <c r="L23" s="10">
         <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="11">
-        <v>0</v>
-      </c>
-      <c r="C24" s="11">
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
         <v>4</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="8">
         <v>4</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="8">
         <v>2</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="8">
         <v>2</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="8">
         <v>9</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="8">
         <v>4</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="8">
         <v>2</v>
       </c>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11">
+      <c r="J24" s="8"/>
+      <c r="K24" s="8">
         <v>7</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="10">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="8">
         <v>6</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="8">
         <v>1</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="E25" s="11">
-        <v>0</v>
-      </c>
-      <c r="F25" s="11">
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
         <v>6</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="8">
         <v>6</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="8">
         <v>3</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="8">
         <v>1</v>
       </c>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11">
+      <c r="J25" s="8"/>
+      <c r="K25" s="8">
         <v>6</v>
       </c>
-      <c r="L25" s="13">
+      <c r="L25" s="10">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8">
         <v>21</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="13">
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="10">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="11">
-        <v>0</v>
-      </c>
-      <c r="C27" s="11">
-        <v>0</v>
-      </c>
-      <c r="D27" s="11">
-        <v>0</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11">
+      <c r="B27" s="8">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8">
         <v>2</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="8">
         <v>4</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="8">
         <v>7</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="8">
         <v>1</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11">
+      <c r="J27" s="8"/>
+      <c r="K27" s="8">
         <v>4</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L27" s="10">
         <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8">
         <v>1</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11">
+      <c r="D28" s="8"/>
+      <c r="E28" s="8">
         <v>1</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="8">
         <v>7</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="8">
         <v>1</v>
       </c>
-      <c r="H28" s="11">
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
-        <v>0</v>
-      </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11">
+      <c r="H28" s="8">
+        <v>0</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0</v>
+      </c>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8">
         <v>5</v>
       </c>
-      <c r="L28" s="13">
+      <c r="L28" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="11">
-        <v>0</v>
-      </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11">
+      <c r="B29" s="8">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8">
         <v>6</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11">
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8">
         <v>1</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11">
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8">
         <v>3</v>
       </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="13">
+      <c r="K29" s="8"/>
+      <c r="L29" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="11">
-        <v>0</v>
-      </c>
-      <c r="C30" s="11">
-        <v>0</v>
-      </c>
-      <c r="D30" s="11">
+      <c r="B30" s="8">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0</v>
+      </c>
+      <c r="D30" s="8">
         <v>1</v>
       </c>
-      <c r="E30" s="11">
-        <v>0</v>
-      </c>
-      <c r="F30" s="11">
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8">
         <v>2</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="8">
         <v>3</v>
       </c>
-      <c r="H30" s="11">
-        <v>0</v>
-      </c>
-      <c r="I30" s="11">
-        <v>0</v>
-      </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11">
-        <v>0</v>
-      </c>
-      <c r="L30" s="13">
+      <c r="H30" s="8">
+        <v>0</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0</v>
+      </c>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8">
+        <v>0</v>
+      </c>
+      <c r="L30" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8">
         <v>1</v>
       </c>
-      <c r="D31" s="11">
-        <v>0</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0</v>
-      </c>
-      <c r="F31" s="11">
-        <v>0</v>
-      </c>
-      <c r="G31" s="11">
-        <v>0</v>
-      </c>
-      <c r="H31" s="11">
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0</v>
+      </c>
+      <c r="H31" s="8">
         <v>3</v>
       </c>
-      <c r="I31" s="11">
-        <v>0</v>
-      </c>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11">
+      <c r="I31" s="8">
+        <v>0</v>
+      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8">
         <v>1</v>
       </c>
-      <c r="L31" s="13">
+      <c r="L31" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="11">
-        <v>0</v>
-      </c>
-      <c r="C32" s="11">
-        <v>0</v>
-      </c>
-      <c r="D32" s="11">
-        <v>0</v>
-      </c>
-      <c r="E32" s="11">
-        <v>0</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11">
+      <c r="B32" s="8">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0</v>
+      </c>
+      <c r="D32" s="8">
+        <v>0</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8">
         <v>1</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="8">
         <v>1</v>
       </c>
-      <c r="I32" s="11">
-        <v>0</v>
-      </c>
-      <c r="J32" s="11">
-        <v>0</v>
-      </c>
-      <c r="K32" s="11"/>
-      <c r="L32" s="13">
+      <c r="I32" s="8">
+        <v>0</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0</v>
+      </c>
+      <c r="K32" s="8"/>
+      <c r="L32" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11">
-        <v>0</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11">
-        <v>0</v>
-      </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8">
+        <v>0</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8">
+        <v>0</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8">
         <v>2</v>
       </c>
-      <c r="I33" s="11">
-        <v>0</v>
-      </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11">
-        <v>0</v>
-      </c>
-      <c r="L33" s="13">
+      <c r="I33" s="8">
+        <v>0</v>
+      </c>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8">
+        <v>0</v>
+      </c>
+      <c r="L33" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="8">
         <v>2</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="13">
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11">
-        <v>0</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11">
-        <v>0</v>
-      </c>
-      <c r="F35" s="11">
-        <v>0</v>
-      </c>
-      <c r="G35" s="11">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8">
+        <v>0</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0</v>
+      </c>
+      <c r="G35" s="8">
         <v>1</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="8">
         <v>1</v>
       </c>
-      <c r="I35" s="11">
-        <v>0</v>
-      </c>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11">
-        <v>0</v>
-      </c>
-      <c r="L35" s="13">
+      <c r="I35" s="8">
+        <v>0</v>
+      </c>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8">
+        <v>0</v>
+      </c>
+      <c r="L35" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11">
-        <v>0</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11">
-        <v>0</v>
-      </c>
-      <c r="G36" s="11">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8">
+        <v>0</v>
+      </c>
+      <c r="G36" s="8">
         <v>1</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11">
-        <v>0</v>
-      </c>
-      <c r="L36" s="13">
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8">
+        <v>0</v>
+      </c>
+      <c r="L36" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11">
-        <v>0</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8">
         <v>1</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="13">
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11">
-        <v>0</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11">
-        <v>0</v>
-      </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8">
+        <v>0</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8">
+        <v>0</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8">
         <v>1</v>
       </c>
-      <c r="I38" s="11">
-        <v>0</v>
-      </c>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11">
-        <v>0</v>
-      </c>
-      <c r="L38" s="13">
+      <c r="I38" s="8">
+        <v>0</v>
+      </c>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8">
+        <v>0</v>
+      </c>
+      <c r="L38" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="8">
         <v>1</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11">
-        <v>0</v>
-      </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11">
-        <v>0</v>
-      </c>
-      <c r="K39" s="11"/>
-      <c r="L39" s="13">
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8">
+        <v>0</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8">
+        <v>0</v>
+      </c>
+      <c r="K39" s="8"/>
+      <c r="L39" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11">
-        <v>0</v>
-      </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11">
-        <v>0</v>
-      </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11">
-        <v>0</v>
-      </c>
-      <c r="I40" s="11">
-        <v>0</v>
-      </c>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11">
-        <v>0</v>
-      </c>
-      <c r="L40" s="13">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8">
+        <v>0</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8">
+        <v>0</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8">
+        <v>0</v>
+      </c>
+      <c r="I40" s="8">
+        <v>0</v>
+      </c>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8">
+        <v>0</v>
+      </c>
+      <c r="L40" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11">
-        <v>0</v>
-      </c>
-      <c r="I41" s="11">
-        <v>0</v>
-      </c>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="13">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8">
+        <v>0</v>
+      </c>
+      <c r="I41" s="8">
+        <v>0</v>
+      </c>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11">
-        <v>0</v>
-      </c>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="13">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8">
+        <v>0</v>
+      </c>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11">
-        <v>0</v>
-      </c>
-      <c r="I43" s="11">
-        <v>0</v>
-      </c>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="13">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8">
+        <v>0</v>
+      </c>
+      <c r="I43" s="8">
+        <v>0</v>
+      </c>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11">
-        <v>0</v>
-      </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11">
-        <v>0</v>
-      </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11">
-        <v>0</v>
-      </c>
-      <c r="I44" s="11">
-        <v>0</v>
-      </c>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11">
-        <v>0</v>
-      </c>
-      <c r="L44" s="13">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8">
+        <v>0</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8">
+        <v>0</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8">
+        <v>0</v>
+      </c>
+      <c r="I44" s="8">
+        <v>0</v>
+      </c>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8">
+        <v>0</v>
+      </c>
+      <c r="L44" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11">
-        <v>0</v>
-      </c>
-      <c r="I45" s="11">
-        <v>0</v>
-      </c>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="13">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8">
+        <v>0</v>
+      </c>
+      <c r="I45" s="8">
+        <v>0</v>
+      </c>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11">
-        <v>0</v>
-      </c>
-      <c r="I46" s="11">
-        <v>0</v>
-      </c>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="13">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8">
+        <v>0</v>
+      </c>
+      <c r="I46" s="8">
+        <v>0</v>
+      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11">
-        <v>0</v>
-      </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11">
-        <v>0</v>
-      </c>
-      <c r="I47" s="11">
-        <v>0</v>
-      </c>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11">
-        <v>0</v>
-      </c>
-      <c r="L47" s="13">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8">
+        <v>0</v>
+      </c>
+      <c r="I47" s="8">
+        <v>0</v>
+      </c>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8">
+        <v>0</v>
+      </c>
+      <c r="L47" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11">
-        <v>0</v>
-      </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11">
-        <v>0</v>
-      </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11">
-        <v>0</v>
-      </c>
-      <c r="I48" s="11">
-        <v>0</v>
-      </c>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="13">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8">
+        <v>0</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8">
+        <v>0</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8">
+        <v>0</v>
+      </c>
+      <c r="I48" s="8">
+        <v>0</v>
+      </c>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11">
-        <v>0</v>
-      </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11">
-        <v>0</v>
-      </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11">
-        <v>0</v>
-      </c>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11">
-        <v>0</v>
-      </c>
-      <c r="L49" s="13">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8">
+        <v>0</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8">
+        <v>0</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8">
+        <v>0</v>
+      </c>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8">
+        <v>0</v>
+      </c>
+      <c r="L49" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11">
-        <v>0</v>
-      </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11">
-        <v>0</v>
-      </c>
-      <c r="F50" s="11">
-        <v>0</v>
-      </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11">
-        <v>0</v>
-      </c>
-      <c r="L50" s="13">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8">
+        <v>0</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8">
+        <v>0</v>
+      </c>
+      <c r="F50" s="8">
+        <v>0</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8">
+        <v>0</v>
+      </c>
+      <c r="L50" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11">
-        <v>0</v>
-      </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11">
-        <v>0</v>
-      </c>
-      <c r="H51" s="11">
-        <v>0</v>
-      </c>
-      <c r="I51" s="11">
-        <v>0</v>
-      </c>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="13">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8">
+        <v>0</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8">
+        <v>0</v>
+      </c>
+      <c r="H51" s="8">
+        <v>0</v>
+      </c>
+      <c r="I51" s="8">
+        <v>0</v>
+      </c>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11">
-        <v>0</v>
-      </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11">
-        <v>0</v>
-      </c>
-      <c r="F52" s="11">
-        <v>0</v>
-      </c>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11">
-        <v>0</v>
-      </c>
-      <c r="I52" s="11">
-        <v>0</v>
-      </c>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11">
-        <v>0</v>
-      </c>
-      <c r="L52" s="13">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8">
+        <v>0</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8">
+        <v>0</v>
+      </c>
+      <c r="F52" s="8">
+        <v>0</v>
+      </c>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8">
+        <v>0</v>
+      </c>
+      <c r="I52" s="8">
+        <v>0</v>
+      </c>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8">
+        <v>0</v>
+      </c>
+      <c r="L52" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11">
-        <v>0</v>
-      </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11">
-        <v>0</v>
-      </c>
-      <c r="F53" s="11">
-        <v>0</v>
-      </c>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11">
-        <v>0</v>
-      </c>
-      <c r="I53" s="11">
-        <v>0</v>
-      </c>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11">
-        <v>0</v>
-      </c>
-      <c r="L53" s="13">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8">
+        <v>0</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8">
+        <v>0</v>
+      </c>
+      <c r="F53" s="8">
+        <v>0</v>
+      </c>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8">
+        <v>0</v>
+      </c>
+      <c r="I53" s="8">
+        <v>0</v>
+      </c>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8">
+        <v>0</v>
+      </c>
+      <c r="L53" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="21" t="s">
+      <c r="A54" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11">
-        <v>0</v>
-      </c>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="13">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8">
+        <v>0</v>
+      </c>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11">
-        <v>0</v>
-      </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11">
-        <v>0</v>
-      </c>
-      <c r="I55" s="11">
-        <v>0</v>
-      </c>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="13">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8">
+        <v>0</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8">
+        <v>0</v>
+      </c>
+      <c r="I55" s="8">
+        <v>0</v>
+      </c>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11">
-        <v>0</v>
-      </c>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11">
-        <v>0</v>
-      </c>
-      <c r="K56" s="11"/>
-      <c r="L56" s="13">
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8">
+        <v>0</v>
+      </c>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8">
+        <v>0</v>
+      </c>
+      <c r="K56" s="8"/>
+      <c r="L56" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11">
-        <v>0</v>
-      </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11">
-        <v>0</v>
-      </c>
-      <c r="F57" s="11">
-        <v>0</v>
-      </c>
-      <c r="G57" s="11">
-        <v>0</v>
-      </c>
-      <c r="H57" s="11">
-        <v>0</v>
-      </c>
-      <c r="I57" s="11">
-        <v>0</v>
-      </c>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11">
-        <v>0</v>
-      </c>
-      <c r="L57" s="13">
+      <c r="B57" s="8"/>
+      <c r="C57" s="8">
+        <v>0</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8">
+        <v>0</v>
+      </c>
+      <c r="F57" s="8">
+        <v>0</v>
+      </c>
+      <c r="G57" s="8">
+        <v>0</v>
+      </c>
+      <c r="H57" s="8">
+        <v>0</v>
+      </c>
+      <c r="I57" s="8">
+        <v>0</v>
+      </c>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8">
+        <v>0</v>
+      </c>
+      <c r="L57" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11">
-        <v>0</v>
-      </c>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="13">
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8">
+        <v>0</v>
+      </c>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11">
-        <v>0</v>
-      </c>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11">
-        <v>0</v>
-      </c>
-      <c r="I59" s="11">
-        <v>0</v>
-      </c>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="13">
+      <c r="B59" s="8"/>
+      <c r="C59" s="8">
+        <v>0</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8">
+        <v>0</v>
+      </c>
+      <c r="I59" s="8">
+        <v>0</v>
+      </c>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="21" t="s">
+      <c r="A60" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11">
-        <v>0</v>
-      </c>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11">
-        <v>0</v>
-      </c>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11">
-        <v>0</v>
-      </c>
-      <c r="I60" s="11">
-        <v>0</v>
-      </c>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="13">
+      <c r="B60" s="8"/>
+      <c r="C60" s="8">
+        <v>0</v>
+      </c>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8">
+        <v>0</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8">
+        <v>0</v>
+      </c>
+      <c r="I60" s="8">
+        <v>0</v>
+      </c>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11">
-        <v>0</v>
-      </c>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11">
-        <v>0</v>
-      </c>
-      <c r="I61" s="11">
-        <v>0</v>
-      </c>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="13">
+      <c r="B61" s="8"/>
+      <c r="C61" s="8">
+        <v>0</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8">
+        <v>0</v>
+      </c>
+      <c r="I61" s="8">
+        <v>0</v>
+      </c>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="21" t="s">
+      <c r="A62" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11">
-        <v>0</v>
-      </c>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11">
-        <v>0</v>
-      </c>
-      <c r="I62" s="11">
-        <v>0</v>
-      </c>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="13">
+      <c r="B62" s="8"/>
+      <c r="C62" s="8">
+        <v>0</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8">
+        <v>0</v>
+      </c>
+      <c r="I62" s="8">
+        <v>0</v>
+      </c>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="21" t="s">
+      <c r="A63" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11">
-        <v>0</v>
-      </c>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11">
-        <v>0</v>
-      </c>
-      <c r="F63" s="11">
-        <v>0</v>
-      </c>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11">
-        <v>0</v>
-      </c>
-      <c r="I63" s="11">
-        <v>0</v>
-      </c>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="13">
+      <c r="B63" s="8"/>
+      <c r="C63" s="8">
+        <v>0</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8">
+        <v>0</v>
+      </c>
+      <c r="F63" s="8">
+        <v>0</v>
+      </c>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8">
+        <v>0</v>
+      </c>
+      <c r="I63" s="8">
+        <v>0</v>
+      </c>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="21" t="s">
+      <c r="A64" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11">
-        <v>0</v>
-      </c>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="13">
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8">
+        <v>0</v>
+      </c>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11">
-        <v>0</v>
-      </c>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11">
-        <v>0</v>
-      </c>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="13">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8">
+        <v>0</v>
+      </c>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8">
+        <v>0</v>
+      </c>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="10">
         <v>0</v>
       </c>
     </row>
@@ -11901,7 +11501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H377"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>